<commit_message>
re-ran template generation script
</commit_message>
<xml_diff>
--- a/publisher/public/assets/DEFENSE.xlsx
+++ b/publisher/public/assets/DEFENSE.xlsx
@@ -22,7 +22,7 @@
     <sheet name="cases_disposed" sheetId="13" r:id="rId13"/>
     <sheet name="cases_disposed_by_type" sheetId="14" r:id="rId14"/>
     <sheet name="cases_disposed_by_race" sheetId="15" r:id="rId15"/>
-    <sheet name="cases_disposed_by_gender" sheetId="16" r:id="rId16"/>
+    <sheet name="cases_disposed_by_sex" sheetId="16" r:id="rId16"/>
     <sheet name="complaints_sustained" sheetId="17" r:id="rId17"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3853" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3709" uniqueCount="79">
   <si>
     <t>year</t>
   </si>
@@ -257,22 +257,16 @@
     <t>Unknown / Unknown Ethnicity</t>
   </si>
   <si>
-    <t>gender</t>
+    <t>biological_sex</t>
   </si>
   <si>
-    <t>Male</t>
+    <t>Male Biological Sex</t>
   </si>
   <si>
-    <t>Female</t>
+    <t>Female Biological Sex</t>
   </si>
   <si>
-    <t>Other</t>
-  </si>
-  <si>
-    <t>Non-Binary</t>
-  </si>
-  <si>
-    <t>Unknown</t>
+    <t>Unknown Biological Sex</t>
   </si>
 </sst>
 </file>
@@ -11526,14 +11520,14 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D121"/>
+  <dimension ref="A1:D73"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="2" width="8.7109375" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="22.7109375" customWidth="1"/>
     <col min="4" max="4" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -11589,10 +11583,10 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C5" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -11600,10 +11594,10 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C6" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -11614,7 +11608,7 @@
         <v>27</v>
       </c>
       <c r="C7" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -11622,10 +11616,10 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -11633,10 +11627,10 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -11644,10 +11638,10 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -11655,10 +11649,10 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C11" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -11666,10 +11660,10 @@
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C12" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -11677,10 +11671,10 @@
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C13" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -11688,10 +11682,10 @@
         <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C14" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -11699,10 +11693,10 @@
         <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C15" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -11710,10 +11704,10 @@
         <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C16" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -11721,7 +11715,7 @@
         <v>2</v>
       </c>
       <c r="B17" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C17" t="s">
         <v>76</v>
@@ -11732,7 +11726,7 @@
         <v>2</v>
       </c>
       <c r="B18" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C18" t="s">
         <v>77</v>
@@ -11743,7 +11737,7 @@
         <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C19" t="s">
         <v>78</v>
@@ -11754,10 +11748,10 @@
         <v>2</v>
       </c>
       <c r="B20" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C20" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -11765,10 +11759,10 @@
         <v>2</v>
       </c>
       <c r="B21" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C21" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -11776,10 +11770,10 @@
         <v>2</v>
       </c>
       <c r="B22" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C22" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -11787,10 +11781,10 @@
         <v>2</v>
       </c>
       <c r="B23" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -11798,10 +11792,10 @@
         <v>2</v>
       </c>
       <c r="B24" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C24" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -11809,10 +11803,10 @@
         <v>2</v>
       </c>
       <c r="B25" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C25" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -11820,10 +11814,10 @@
         <v>2</v>
       </c>
       <c r="B26" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C26" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -11831,10 +11825,10 @@
         <v>2</v>
       </c>
       <c r="B27" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C27" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -11842,10 +11836,10 @@
         <v>2</v>
       </c>
       <c r="B28" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C28" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -11853,10 +11847,10 @@
         <v>2</v>
       </c>
       <c r="B29" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C29" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -11864,10 +11858,10 @@
         <v>2</v>
       </c>
       <c r="B30" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C30" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -11875,10 +11869,10 @@
         <v>2</v>
       </c>
       <c r="B31" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C31" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -11886,7 +11880,7 @@
         <v>2</v>
       </c>
       <c r="B32" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C32" t="s">
         <v>76</v>
@@ -11897,7 +11891,7 @@
         <v>2</v>
       </c>
       <c r="B33" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C33" t="s">
         <v>77</v>
@@ -11908,7 +11902,7 @@
         <v>2</v>
       </c>
       <c r="B34" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C34" t="s">
         <v>78</v>
@@ -11919,10 +11913,10 @@
         <v>2</v>
       </c>
       <c r="B35" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C35" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -11930,10 +11924,10 @@
         <v>2</v>
       </c>
       <c r="B36" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C36" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -11941,117 +11935,117 @@
         <v>2</v>
       </c>
       <c r="B37" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C37" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B38" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C38" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B39" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C39" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B40" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C40" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B41" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C41" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B42" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C42" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B43" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C43" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B44" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C44" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B45" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C45" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B46" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C46" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B47" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C47" t="s">
         <v>76</v>
@@ -12059,10 +12053,10 @@
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B48" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C48" t="s">
         <v>77</v>
@@ -12070,10 +12064,10 @@
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B49" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C49" t="s">
         <v>78</v>
@@ -12081,134 +12075,134 @@
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B50" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C50" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B51" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C51" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B52" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C52" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B53" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C53" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B54" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C54" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B55" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C55" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B56" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C56" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B57" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C57" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B58" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C58" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B59" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C59" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B60" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C60" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B61" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C61" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="62" spans="1:3">
@@ -12216,7 +12210,7 @@
         <v>3</v>
       </c>
       <c r="B62" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="C62" t="s">
         <v>76</v>
@@ -12227,7 +12221,7 @@
         <v>3</v>
       </c>
       <c r="B63" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="C63" t="s">
         <v>77</v>
@@ -12238,7 +12232,7 @@
         <v>3</v>
       </c>
       <c r="B64" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="C64" t="s">
         <v>78</v>
@@ -12249,10 +12243,10 @@
         <v>3</v>
       </c>
       <c r="B65" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="C65" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="66" spans="1:3">
@@ -12260,10 +12254,10 @@
         <v>3</v>
       </c>
       <c r="B66" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="C66" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="67" spans="1:3">
@@ -12271,10 +12265,10 @@
         <v>3</v>
       </c>
       <c r="B67" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="C67" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="68" spans="1:3">
@@ -12282,10 +12276,10 @@
         <v>3</v>
       </c>
       <c r="B68" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="C68" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="69" spans="1:3">
@@ -12293,10 +12287,10 @@
         <v>3</v>
       </c>
       <c r="B69" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="C69" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="70" spans="1:3">
@@ -12304,10 +12298,10 @@
         <v>3</v>
       </c>
       <c r="B70" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="C70" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="71" spans="1:3">
@@ -12315,10 +12309,10 @@
         <v>3</v>
       </c>
       <c r="B71" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="C71" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="72" spans="1:3">
@@ -12326,10 +12320,10 @@
         <v>3</v>
       </c>
       <c r="B72" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="C72" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="73" spans="1:3">
@@ -12337,538 +12331,10 @@
         <v>3</v>
       </c>
       <c r="B73" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="C73" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3">
-      <c r="A74" t="s">
-        <v>3</v>
-      </c>
-      <c r="B74" t="s">
-        <v>28</v>
-      </c>
-      <c r="C74" t="s">
         <v>78</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3">
-      <c r="A75" t="s">
-        <v>3</v>
-      </c>
-      <c r="B75" t="s">
-        <v>28</v>
-      </c>
-      <c r="C75" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3">
-      <c r="A76" t="s">
-        <v>3</v>
-      </c>
-      <c r="B76" t="s">
-        <v>28</v>
-      </c>
-      <c r="C76" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3">
-      <c r="A77" t="s">
-        <v>3</v>
-      </c>
-      <c r="B77" t="s">
-        <v>29</v>
-      </c>
-      <c r="C77" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3">
-      <c r="A78" t="s">
-        <v>3</v>
-      </c>
-      <c r="B78" t="s">
-        <v>29</v>
-      </c>
-      <c r="C78" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3">
-      <c r="A79" t="s">
-        <v>3</v>
-      </c>
-      <c r="B79" t="s">
-        <v>29</v>
-      </c>
-      <c r="C79" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3">
-      <c r="A80" t="s">
-        <v>3</v>
-      </c>
-      <c r="B80" t="s">
-        <v>29</v>
-      </c>
-      <c r="C80" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3">
-      <c r="A81" t="s">
-        <v>3</v>
-      </c>
-      <c r="B81" t="s">
-        <v>29</v>
-      </c>
-      <c r="C81" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3">
-      <c r="A82" t="s">
-        <v>3</v>
-      </c>
-      <c r="B82" t="s">
-        <v>30</v>
-      </c>
-      <c r="C82" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3">
-      <c r="A83" t="s">
-        <v>3</v>
-      </c>
-      <c r="B83" t="s">
-        <v>30</v>
-      </c>
-      <c r="C83" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3">
-      <c r="A84" t="s">
-        <v>3</v>
-      </c>
-      <c r="B84" t="s">
-        <v>30</v>
-      </c>
-      <c r="C84" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3">
-      <c r="A85" t="s">
-        <v>3</v>
-      </c>
-      <c r="B85" t="s">
-        <v>30</v>
-      </c>
-      <c r="C85" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3">
-      <c r="A86" t="s">
-        <v>3</v>
-      </c>
-      <c r="B86" t="s">
-        <v>30</v>
-      </c>
-      <c r="C86" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3">
-      <c r="A87" t="s">
-        <v>3</v>
-      </c>
-      <c r="B87" t="s">
-        <v>31</v>
-      </c>
-      <c r="C87" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3">
-      <c r="A88" t="s">
-        <v>3</v>
-      </c>
-      <c r="B88" t="s">
-        <v>31</v>
-      </c>
-      <c r="C88" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3">
-      <c r="A89" t="s">
-        <v>3</v>
-      </c>
-      <c r="B89" t="s">
-        <v>31</v>
-      </c>
-      <c r="C89" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3">
-      <c r="A90" t="s">
-        <v>3</v>
-      </c>
-      <c r="B90" t="s">
-        <v>31</v>
-      </c>
-      <c r="C90" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3">
-      <c r="A91" t="s">
-        <v>3</v>
-      </c>
-      <c r="B91" t="s">
-        <v>31</v>
-      </c>
-      <c r="C91" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3">
-      <c r="A92" t="s">
-        <v>3</v>
-      </c>
-      <c r="B92" t="s">
-        <v>32</v>
-      </c>
-      <c r="C92" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3">
-      <c r="A93" t="s">
-        <v>3</v>
-      </c>
-      <c r="B93" t="s">
-        <v>32</v>
-      </c>
-      <c r="C93" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3">
-      <c r="A94" t="s">
-        <v>3</v>
-      </c>
-      <c r="B94" t="s">
-        <v>32</v>
-      </c>
-      <c r="C94" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3">
-      <c r="A95" t="s">
-        <v>3</v>
-      </c>
-      <c r="B95" t="s">
-        <v>32</v>
-      </c>
-      <c r="C95" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3">
-      <c r="A96" t="s">
-        <v>3</v>
-      </c>
-      <c r="B96" t="s">
-        <v>32</v>
-      </c>
-      <c r="C96" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3">
-      <c r="A97" t="s">
-        <v>3</v>
-      </c>
-      <c r="B97" t="s">
-        <v>33</v>
-      </c>
-      <c r="C97" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3">
-      <c r="A98" t="s">
-        <v>3</v>
-      </c>
-      <c r="B98" t="s">
-        <v>33</v>
-      </c>
-      <c r="C98" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3">
-      <c r="A99" t="s">
-        <v>3</v>
-      </c>
-      <c r="B99" t="s">
-        <v>33</v>
-      </c>
-      <c r="C99" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3">
-      <c r="A100" t="s">
-        <v>3</v>
-      </c>
-      <c r="B100" t="s">
-        <v>33</v>
-      </c>
-      <c r="C100" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3">
-      <c r="A101" t="s">
-        <v>3</v>
-      </c>
-      <c r="B101" t="s">
-        <v>33</v>
-      </c>
-      <c r="C101" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3">
-      <c r="A102" t="s">
-        <v>3</v>
-      </c>
-      <c r="B102" t="s">
-        <v>34</v>
-      </c>
-      <c r="C102" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3">
-      <c r="A103" t="s">
-        <v>3</v>
-      </c>
-      <c r="B103" t="s">
-        <v>34</v>
-      </c>
-      <c r="C103" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3">
-      <c r="A104" t="s">
-        <v>3</v>
-      </c>
-      <c r="B104" t="s">
-        <v>34</v>
-      </c>
-      <c r="C104" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3">
-      <c r="A105" t="s">
-        <v>3</v>
-      </c>
-      <c r="B105" t="s">
-        <v>34</v>
-      </c>
-      <c r="C105" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3">
-      <c r="A106" t="s">
-        <v>3</v>
-      </c>
-      <c r="B106" t="s">
-        <v>34</v>
-      </c>
-      <c r="C106" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3">
-      <c r="A107" t="s">
-        <v>3</v>
-      </c>
-      <c r="B107" t="s">
-        <v>35</v>
-      </c>
-      <c r="C107" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3">
-      <c r="A108" t="s">
-        <v>3</v>
-      </c>
-      <c r="B108" t="s">
-        <v>35</v>
-      </c>
-      <c r="C108" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3">
-      <c r="A109" t="s">
-        <v>3</v>
-      </c>
-      <c r="B109" t="s">
-        <v>35</v>
-      </c>
-      <c r="C109" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3">
-      <c r="A110" t="s">
-        <v>3</v>
-      </c>
-      <c r="B110" t="s">
-        <v>35</v>
-      </c>
-      <c r="C110" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3">
-      <c r="A111" t="s">
-        <v>3</v>
-      </c>
-      <c r="B111" t="s">
-        <v>35</v>
-      </c>
-      <c r="C111" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3">
-      <c r="A112" t="s">
-        <v>3</v>
-      </c>
-      <c r="B112" t="s">
-        <v>36</v>
-      </c>
-      <c r="C112" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3">
-      <c r="A113" t="s">
-        <v>3</v>
-      </c>
-      <c r="B113" t="s">
-        <v>36</v>
-      </c>
-      <c r="C113" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3">
-      <c r="A114" t="s">
-        <v>3</v>
-      </c>
-      <c r="B114" t="s">
-        <v>36</v>
-      </c>
-      <c r="C114" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3">
-      <c r="A115" t="s">
-        <v>3</v>
-      </c>
-      <c r="B115" t="s">
-        <v>36</v>
-      </c>
-      <c r="C115" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3">
-      <c r="A116" t="s">
-        <v>3</v>
-      </c>
-      <c r="B116" t="s">
-        <v>36</v>
-      </c>
-      <c r="C116" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3">
-      <c r="A117" t="s">
-        <v>3</v>
-      </c>
-      <c r="B117" t="s">
-        <v>37</v>
-      </c>
-      <c r="C117" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3">
-      <c r="A118" t="s">
-        <v>3</v>
-      </c>
-      <c r="B118" t="s">
-        <v>37</v>
-      </c>
-      <c r="C118" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3">
-      <c r="A119" t="s">
-        <v>3</v>
-      </c>
-      <c r="B119" t="s">
-        <v>37</v>
-      </c>
-      <c r="C119" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3">
-      <c r="A120" t="s">
-        <v>3</v>
-      </c>
-      <c r="B120" t="s">
-        <v>37</v>
-      </c>
-      <c r="C120" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3">
-      <c r="A121" t="s">
-        <v>3</v>
-      </c>
-      <c r="B121" t="s">
-        <v>37</v>
-      </c>
-      <c r="C121" t="s">
-        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
re-ran template generation script (#576)
</commit_message>
<xml_diff>
--- a/publisher/public/assets/DEFENSE.xlsx
+++ b/publisher/public/assets/DEFENSE.xlsx
@@ -22,7 +22,7 @@
     <sheet name="cases_disposed" sheetId="13" r:id="rId13"/>
     <sheet name="cases_disposed_by_type" sheetId="14" r:id="rId14"/>
     <sheet name="cases_disposed_by_race" sheetId="15" r:id="rId15"/>
-    <sheet name="cases_disposed_by_gender" sheetId="16" r:id="rId16"/>
+    <sheet name="cases_disposed_by_sex" sheetId="16" r:id="rId16"/>
     <sheet name="complaints_sustained" sheetId="17" r:id="rId17"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3853" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3709" uniqueCount="79">
   <si>
     <t>year</t>
   </si>
@@ -257,22 +257,16 @@
     <t>Unknown / Unknown Ethnicity</t>
   </si>
   <si>
-    <t>gender</t>
+    <t>biological_sex</t>
   </si>
   <si>
-    <t>Male</t>
+    <t>Male Biological Sex</t>
   </si>
   <si>
-    <t>Female</t>
+    <t>Female Biological Sex</t>
   </si>
   <si>
-    <t>Other</t>
-  </si>
-  <si>
-    <t>Non-Binary</t>
-  </si>
-  <si>
-    <t>Unknown</t>
+    <t>Unknown Biological Sex</t>
   </si>
 </sst>
 </file>
@@ -11526,14 +11520,14 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D121"/>
+  <dimension ref="A1:D73"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="2" width="8.7109375" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="22.7109375" customWidth="1"/>
     <col min="4" max="4" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -11589,10 +11583,10 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C5" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -11600,10 +11594,10 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C6" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -11614,7 +11608,7 @@
         <v>27</v>
       </c>
       <c r="C7" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -11622,10 +11616,10 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -11633,10 +11627,10 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -11644,10 +11638,10 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -11655,10 +11649,10 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C11" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -11666,10 +11660,10 @@
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C12" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -11677,10 +11671,10 @@
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C13" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -11688,10 +11682,10 @@
         <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C14" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -11699,10 +11693,10 @@
         <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C15" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -11710,10 +11704,10 @@
         <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C16" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -11721,7 +11715,7 @@
         <v>2</v>
       </c>
       <c r="B17" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C17" t="s">
         <v>76</v>
@@ -11732,7 +11726,7 @@
         <v>2</v>
       </c>
       <c r="B18" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C18" t="s">
         <v>77</v>
@@ -11743,7 +11737,7 @@
         <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C19" t="s">
         <v>78</v>
@@ -11754,10 +11748,10 @@
         <v>2</v>
       </c>
       <c r="B20" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C20" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -11765,10 +11759,10 @@
         <v>2</v>
       </c>
       <c r="B21" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C21" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -11776,10 +11770,10 @@
         <v>2</v>
       </c>
       <c r="B22" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C22" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -11787,10 +11781,10 @@
         <v>2</v>
       </c>
       <c r="B23" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -11798,10 +11792,10 @@
         <v>2</v>
       </c>
       <c r="B24" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C24" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -11809,10 +11803,10 @@
         <v>2</v>
       </c>
       <c r="B25" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C25" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -11820,10 +11814,10 @@
         <v>2</v>
       </c>
       <c r="B26" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C26" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -11831,10 +11825,10 @@
         <v>2</v>
       </c>
       <c r="B27" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C27" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -11842,10 +11836,10 @@
         <v>2</v>
       </c>
       <c r="B28" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C28" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -11853,10 +11847,10 @@
         <v>2</v>
       </c>
       <c r="B29" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C29" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -11864,10 +11858,10 @@
         <v>2</v>
       </c>
       <c r="B30" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C30" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -11875,10 +11869,10 @@
         <v>2</v>
       </c>
       <c r="B31" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C31" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -11886,7 +11880,7 @@
         <v>2</v>
       </c>
       <c r="B32" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C32" t="s">
         <v>76</v>
@@ -11897,7 +11891,7 @@
         <v>2</v>
       </c>
       <c r="B33" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C33" t="s">
         <v>77</v>
@@ -11908,7 +11902,7 @@
         <v>2</v>
       </c>
       <c r="B34" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C34" t="s">
         <v>78</v>
@@ -11919,10 +11913,10 @@
         <v>2</v>
       </c>
       <c r="B35" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C35" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -11930,10 +11924,10 @@
         <v>2</v>
       </c>
       <c r="B36" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C36" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -11941,117 +11935,117 @@
         <v>2</v>
       </c>
       <c r="B37" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C37" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B38" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C38" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B39" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C39" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B40" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C40" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B41" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C41" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B42" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C42" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B43" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C43" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B44" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C44" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B45" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C45" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B46" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C46" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B47" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C47" t="s">
         <v>76</v>
@@ -12059,10 +12053,10 @@
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B48" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C48" t="s">
         <v>77</v>
@@ -12070,10 +12064,10 @@
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B49" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C49" t="s">
         <v>78</v>
@@ -12081,134 +12075,134 @@
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B50" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C50" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B51" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C51" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B52" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C52" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B53" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C53" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B54" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C54" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B55" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C55" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B56" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C56" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B57" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C57" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B58" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C58" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B59" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C59" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B60" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C60" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B61" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C61" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="62" spans="1:3">
@@ -12216,7 +12210,7 @@
         <v>3</v>
       </c>
       <c r="B62" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="C62" t="s">
         <v>76</v>
@@ -12227,7 +12221,7 @@
         <v>3</v>
       </c>
       <c r="B63" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="C63" t="s">
         <v>77</v>
@@ -12238,7 +12232,7 @@
         <v>3</v>
       </c>
       <c r="B64" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="C64" t="s">
         <v>78</v>
@@ -12249,10 +12243,10 @@
         <v>3</v>
       </c>
       <c r="B65" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="C65" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="66" spans="1:3">
@@ -12260,10 +12254,10 @@
         <v>3</v>
       </c>
       <c r="B66" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="C66" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="67" spans="1:3">
@@ -12271,10 +12265,10 @@
         <v>3</v>
       </c>
       <c r="B67" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="C67" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="68" spans="1:3">
@@ -12282,10 +12276,10 @@
         <v>3</v>
       </c>
       <c r="B68" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="C68" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="69" spans="1:3">
@@ -12293,10 +12287,10 @@
         <v>3</v>
       </c>
       <c r="B69" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="C69" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="70" spans="1:3">
@@ -12304,10 +12298,10 @@
         <v>3</v>
       </c>
       <c r="B70" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="C70" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="71" spans="1:3">
@@ -12315,10 +12309,10 @@
         <v>3</v>
       </c>
       <c r="B71" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="C71" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="72" spans="1:3">
@@ -12326,10 +12320,10 @@
         <v>3</v>
       </c>
       <c r="B72" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="C72" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="73" spans="1:3">
@@ -12337,538 +12331,10 @@
         <v>3</v>
       </c>
       <c r="B73" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="C73" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3">
-      <c r="A74" t="s">
-        <v>3</v>
-      </c>
-      <c r="B74" t="s">
-        <v>28</v>
-      </c>
-      <c r="C74" t="s">
         <v>78</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3">
-      <c r="A75" t="s">
-        <v>3</v>
-      </c>
-      <c r="B75" t="s">
-        <v>28</v>
-      </c>
-      <c r="C75" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3">
-      <c r="A76" t="s">
-        <v>3</v>
-      </c>
-      <c r="B76" t="s">
-        <v>28</v>
-      </c>
-      <c r="C76" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3">
-      <c r="A77" t="s">
-        <v>3</v>
-      </c>
-      <c r="B77" t="s">
-        <v>29</v>
-      </c>
-      <c r="C77" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3">
-      <c r="A78" t="s">
-        <v>3</v>
-      </c>
-      <c r="B78" t="s">
-        <v>29</v>
-      </c>
-      <c r="C78" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3">
-      <c r="A79" t="s">
-        <v>3</v>
-      </c>
-      <c r="B79" t="s">
-        <v>29</v>
-      </c>
-      <c r="C79" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3">
-      <c r="A80" t="s">
-        <v>3</v>
-      </c>
-      <c r="B80" t="s">
-        <v>29</v>
-      </c>
-      <c r="C80" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3">
-      <c r="A81" t="s">
-        <v>3</v>
-      </c>
-      <c r="B81" t="s">
-        <v>29</v>
-      </c>
-      <c r="C81" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3">
-      <c r="A82" t="s">
-        <v>3</v>
-      </c>
-      <c r="B82" t="s">
-        <v>30</v>
-      </c>
-      <c r="C82" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3">
-      <c r="A83" t="s">
-        <v>3</v>
-      </c>
-      <c r="B83" t="s">
-        <v>30</v>
-      </c>
-      <c r="C83" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3">
-      <c r="A84" t="s">
-        <v>3</v>
-      </c>
-      <c r="B84" t="s">
-        <v>30</v>
-      </c>
-      <c r="C84" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3">
-      <c r="A85" t="s">
-        <v>3</v>
-      </c>
-      <c r="B85" t="s">
-        <v>30</v>
-      </c>
-      <c r="C85" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3">
-      <c r="A86" t="s">
-        <v>3</v>
-      </c>
-      <c r="B86" t="s">
-        <v>30</v>
-      </c>
-      <c r="C86" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3">
-      <c r="A87" t="s">
-        <v>3</v>
-      </c>
-      <c r="B87" t="s">
-        <v>31</v>
-      </c>
-      <c r="C87" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3">
-      <c r="A88" t="s">
-        <v>3</v>
-      </c>
-      <c r="B88" t="s">
-        <v>31</v>
-      </c>
-      <c r="C88" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3">
-      <c r="A89" t="s">
-        <v>3</v>
-      </c>
-      <c r="B89" t="s">
-        <v>31</v>
-      </c>
-      <c r="C89" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3">
-      <c r="A90" t="s">
-        <v>3</v>
-      </c>
-      <c r="B90" t="s">
-        <v>31</v>
-      </c>
-      <c r="C90" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3">
-      <c r="A91" t="s">
-        <v>3</v>
-      </c>
-      <c r="B91" t="s">
-        <v>31</v>
-      </c>
-      <c r="C91" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3">
-      <c r="A92" t="s">
-        <v>3</v>
-      </c>
-      <c r="B92" t="s">
-        <v>32</v>
-      </c>
-      <c r="C92" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3">
-      <c r="A93" t="s">
-        <v>3</v>
-      </c>
-      <c r="B93" t="s">
-        <v>32</v>
-      </c>
-      <c r="C93" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3">
-      <c r="A94" t="s">
-        <v>3</v>
-      </c>
-      <c r="B94" t="s">
-        <v>32</v>
-      </c>
-      <c r="C94" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3">
-      <c r="A95" t="s">
-        <v>3</v>
-      </c>
-      <c r="B95" t="s">
-        <v>32</v>
-      </c>
-      <c r="C95" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3">
-      <c r="A96" t="s">
-        <v>3</v>
-      </c>
-      <c r="B96" t="s">
-        <v>32</v>
-      </c>
-      <c r="C96" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3">
-      <c r="A97" t="s">
-        <v>3</v>
-      </c>
-      <c r="B97" t="s">
-        <v>33</v>
-      </c>
-      <c r="C97" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3">
-      <c r="A98" t="s">
-        <v>3</v>
-      </c>
-      <c r="B98" t="s">
-        <v>33</v>
-      </c>
-      <c r="C98" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3">
-      <c r="A99" t="s">
-        <v>3</v>
-      </c>
-      <c r="B99" t="s">
-        <v>33</v>
-      </c>
-      <c r="C99" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3">
-      <c r="A100" t="s">
-        <v>3</v>
-      </c>
-      <c r="B100" t="s">
-        <v>33</v>
-      </c>
-      <c r="C100" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3">
-      <c r="A101" t="s">
-        <v>3</v>
-      </c>
-      <c r="B101" t="s">
-        <v>33</v>
-      </c>
-      <c r="C101" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3">
-      <c r="A102" t="s">
-        <v>3</v>
-      </c>
-      <c r="B102" t="s">
-        <v>34</v>
-      </c>
-      <c r="C102" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3">
-      <c r="A103" t="s">
-        <v>3</v>
-      </c>
-      <c r="B103" t="s">
-        <v>34</v>
-      </c>
-      <c r="C103" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3">
-      <c r="A104" t="s">
-        <v>3</v>
-      </c>
-      <c r="B104" t="s">
-        <v>34</v>
-      </c>
-      <c r="C104" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3">
-      <c r="A105" t="s">
-        <v>3</v>
-      </c>
-      <c r="B105" t="s">
-        <v>34</v>
-      </c>
-      <c r="C105" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3">
-      <c r="A106" t="s">
-        <v>3</v>
-      </c>
-      <c r="B106" t="s">
-        <v>34</v>
-      </c>
-      <c r="C106" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3">
-      <c r="A107" t="s">
-        <v>3</v>
-      </c>
-      <c r="B107" t="s">
-        <v>35</v>
-      </c>
-      <c r="C107" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3">
-      <c r="A108" t="s">
-        <v>3</v>
-      </c>
-      <c r="B108" t="s">
-        <v>35</v>
-      </c>
-      <c r="C108" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3">
-      <c r="A109" t="s">
-        <v>3</v>
-      </c>
-      <c r="B109" t="s">
-        <v>35</v>
-      </c>
-      <c r="C109" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3">
-      <c r="A110" t="s">
-        <v>3</v>
-      </c>
-      <c r="B110" t="s">
-        <v>35</v>
-      </c>
-      <c r="C110" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3">
-      <c r="A111" t="s">
-        <v>3</v>
-      </c>
-      <c r="B111" t="s">
-        <v>35</v>
-      </c>
-      <c r="C111" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3">
-      <c r="A112" t="s">
-        <v>3</v>
-      </c>
-      <c r="B112" t="s">
-        <v>36</v>
-      </c>
-      <c r="C112" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3">
-      <c r="A113" t="s">
-        <v>3</v>
-      </c>
-      <c r="B113" t="s">
-        <v>36</v>
-      </c>
-      <c r="C113" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3">
-      <c r="A114" t="s">
-        <v>3</v>
-      </c>
-      <c r="B114" t="s">
-        <v>36</v>
-      </c>
-      <c r="C114" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3">
-      <c r="A115" t="s">
-        <v>3</v>
-      </c>
-      <c r="B115" t="s">
-        <v>36</v>
-      </c>
-      <c r="C115" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3">
-      <c r="A116" t="s">
-        <v>3</v>
-      </c>
-      <c r="B116" t="s">
-        <v>36</v>
-      </c>
-      <c r="C116" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3">
-      <c r="A117" t="s">
-        <v>3</v>
-      </c>
-      <c r="B117" t="s">
-        <v>37</v>
-      </c>
-      <c r="C117" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3">
-      <c r="A118" t="s">
-        <v>3</v>
-      </c>
-      <c r="B118" t="s">
-        <v>37</v>
-      </c>
-      <c r="C118" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3">
-      <c r="A119" t="s">
-        <v>3</v>
-      </c>
-      <c r="B119" t="s">
-        <v>37</v>
-      </c>
-      <c r="C119" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3">
-      <c r="A120" t="s">
-        <v>3</v>
-      </c>
-      <c r="B120" t="s">
-        <v>37</v>
-      </c>
-      <c r="C120" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3">
-      <c r="A121" t="s">
-        <v>3</v>
-      </c>
-      <c r="B121" t="s">
-        <v>37</v>
-      </c>
-      <c r="C121" t="s">
-        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>